<commit_message>
added footprints, fault detection and temperature calc
</commit_message>
<xml_diff>
--- a/driver_module_calc.xlsx
+++ b/driver_module_calc.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Studia\2stp\3SEM\MOC_CZE\HW\TEMiWCZ_BLDC_HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B803F9A9-14B4-49D7-B1DF-F7DA368F16B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3C8443-45FB-4E26-B936-96B3791BE765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="temp" sheetId="2" r:id="rId2"/>
+    <sheet name="current meas" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Qg</t>
   </si>
@@ -162,13 +167,67 @@
   </si>
   <si>
     <t>Ig</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>kOhm</t>
+  </si>
+  <si>
+    <t>uout</t>
+  </si>
+  <si>
+    <t>dout</t>
+  </si>
+  <si>
+    <t>Rt</t>
+  </si>
+  <si>
+    <t>vcc</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>temp ed</t>
+  </si>
+  <si>
+    <t>umax</t>
+  </si>
+  <si>
+    <t>gain</t>
+  </si>
+  <si>
+    <t>min volt diff</t>
+  </si>
+  <si>
+    <t>min i diff</t>
+  </si>
+  <si>
+    <t>min dif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +236,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -322,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -341,7 +408,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -358,6 +426,1411 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Arkusz1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]Arkusz1!$G$2:$G$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Arkusz1!$J$2:$J$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>3.2352384479134706</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2128946372542524</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1844137103615688</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1486438299697053</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1043930865505431</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0504940831543346</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9858885422966739</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9097283274643</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.821484674233258</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.7210526315789472</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6088341118192102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4857822012261335</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3533928041709387</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2136374729238422</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0688419873731188</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9215260518459123</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7742271052871876</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.629333375578784</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4889475674422539</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3547945752429937</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2281771204394902</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1099749155794145</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0006775400942014</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90043908555385799</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.80914320318389032</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.72646941583618996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.65195440459246712</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.58504469291222438</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.52513932143561037</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.47162261141513984</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.42388800956189304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F57-431E-A556-EBDC17E6E027}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="824064800"/>
+        <c:axId val="824066720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="824064800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Temp</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.49126100201330253"/>
+              <c:y val="0.89149052020671327"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="824066720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="824066720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Uout</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="824064800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B96CE1-3169-4D50-967F-0A05F996462E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Arkusz1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="J1" t="str">
+            <v>uout</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>-20</v>
+          </cell>
+          <cell r="J2">
+            <v>3.2352384479134706</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-15</v>
+          </cell>
+          <cell r="J3">
+            <v>3.2128946372542524</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="G4">
+            <v>-10</v>
+          </cell>
+          <cell r="J4">
+            <v>3.1844137103615688</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="G5">
+            <v>-5</v>
+          </cell>
+          <cell r="J5">
+            <v>3.1486438299697053</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="G6">
+            <v>0</v>
+          </cell>
+          <cell r="J6">
+            <v>3.1043930865505431</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="G7">
+            <v>5</v>
+          </cell>
+          <cell r="J7">
+            <v>3.0504940831543346</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="G8">
+            <v>10</v>
+          </cell>
+          <cell r="J8">
+            <v>2.9858885422966739</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="G9">
+            <v>15</v>
+          </cell>
+          <cell r="J9">
+            <v>2.9097283274643</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="G10">
+            <v>20</v>
+          </cell>
+          <cell r="J10">
+            <v>2.821484674233258</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="G11">
+            <v>25</v>
+          </cell>
+          <cell r="J11">
+            <v>2.7210526315789472</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="G12">
+            <v>30</v>
+          </cell>
+          <cell r="J12">
+            <v>2.6088341118192102</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="G13">
+            <v>35</v>
+          </cell>
+          <cell r="J13">
+            <v>2.4857822012261335</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="G14">
+            <v>40</v>
+          </cell>
+          <cell r="J14">
+            <v>2.3533928041709387</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="G15">
+            <v>45</v>
+          </cell>
+          <cell r="J15">
+            <v>2.2136374729238422</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="G16">
+            <v>50</v>
+          </cell>
+          <cell r="J16">
+            <v>2.0688419873731188</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="G17">
+            <v>55</v>
+          </cell>
+          <cell r="J17">
+            <v>1.9215260518459123</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="G18">
+            <v>60</v>
+          </cell>
+          <cell r="J18">
+            <v>1.7742271052871876</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="G19">
+            <v>65</v>
+          </cell>
+          <cell r="J19">
+            <v>1.629333375578784</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="G20">
+            <v>70</v>
+          </cell>
+          <cell r="J20">
+            <v>1.4889475674422539</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="G21">
+            <v>75</v>
+          </cell>
+          <cell r="J21">
+            <v>1.3547945752429937</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="G22">
+            <v>80</v>
+          </cell>
+          <cell r="J22">
+            <v>1.2281771204394902</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="G23">
+            <v>85</v>
+          </cell>
+          <cell r="J23">
+            <v>1.1099749155794145</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="G24">
+            <v>90</v>
+          </cell>
+          <cell r="J24">
+            <v>1.0006775400942014</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="G25">
+            <v>95</v>
+          </cell>
+          <cell r="J25">
+            <v>0.90043908555385799</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="G26">
+            <v>100</v>
+          </cell>
+          <cell r="J26">
+            <v>0.80914320318389032</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="G27">
+            <v>105</v>
+          </cell>
+          <cell r="J27">
+            <v>0.72646941583618996</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="G28">
+            <v>110</v>
+          </cell>
+          <cell r="J28">
+            <v>0.65195440459246712</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="G29">
+            <v>115</v>
+          </cell>
+          <cell r="J29">
+            <v>0.58504469291222438</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="G30">
+            <v>120</v>
+          </cell>
+          <cell r="J30">
+            <v>0.52513932143561037</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="G31">
+            <v>125</v>
+          </cell>
+          <cell r="J31">
+            <v>0.47162261141513984</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="G32">
+            <v>130</v>
+          </cell>
+          <cell r="J32">
+            <v>0.42388800956189304</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +2369,7 @@
       <c r="K16" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16">
         <f>I15/I16</f>
         <v>1.5499999999999998</v>
       </c>
@@ -907,6 +2380,892 @@
       </c>
       <c r="C21" t="s">
         <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77441156-81CB-46C4-9854-CFE67F82DA4A}">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1">
+        <v>47000</v>
+      </c>
+      <c r="G2">
+        <v>-20</v>
+      </c>
+      <c r="H2" s="1">
+        <f>$B$2*EXP($B$6*(1/(G2+273)-1/($B$7+273)))</f>
+        <v>499561.59846057848</v>
+      </c>
+      <c r="I2">
+        <f>H2/1000</f>
+        <v>499.56159846057847</v>
+      </c>
+      <c r="J2" s="18">
+        <f>$B$3*H2/($B$1+H2)</f>
+        <v>3.2352384479134706</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>3.3</v>
+      </c>
+      <c r="G3">
+        <v>-15</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H32" si="0">$B$2*EXP($B$6*(1/(G3+273)-1/($B$7+273)))</f>
+        <v>368851.53060350643</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I32" si="1">H3/1000</f>
+        <v>368.85153060350643</v>
+      </c>
+      <c r="J3" s="18">
+        <f t="shared" ref="J3:J32" si="2">$B$3*H3/($B$1+H3)</f>
+        <v>3.2128946372542524</v>
+      </c>
+      <c r="K3" s="18">
+        <f>ABS(J3-J2)</f>
+        <v>2.23438106592182E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1">
+        <f>B3/(B1+B2)</f>
+        <v>5.789473684210526E-5</v>
+      </c>
+      <c r="C4">
+        <f>B4*1000</f>
+        <v>5.7894736842105263E-2</v>
+      </c>
+      <c r="G4">
+        <v>-10</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>275500.98894279118</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>275.5009889427912</v>
+      </c>
+      <c r="J4" s="18">
+        <f t="shared" si="2"/>
+        <v>3.1844137103615688</v>
+      </c>
+      <c r="K4" s="18">
+        <f t="shared" ref="K4:K32" si="3">ABS(J4-J3)</f>
+        <v>2.8480926892683556E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <f>B4*B2</f>
+        <v>2.7210526315789472</v>
+      </c>
+      <c r="G5">
+        <v>-5</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>208028.7727510212</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>208.02877275102119</v>
+      </c>
+      <c r="J5" s="18">
+        <f t="shared" si="2"/>
+        <v>3.1486438299697053</v>
+      </c>
+      <c r="K5" s="18">
+        <f t="shared" si="3"/>
+        <v>3.5769880391863573E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>3960</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>158705.69356704748</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>158.70569356704749</v>
+      </c>
+      <c r="J6" s="18">
+        <f t="shared" si="2"/>
+        <v>3.1043930865505431</v>
+      </c>
+      <c r="K6" s="18">
+        <f t="shared" si="3"/>
+        <v>4.4250743419162131E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>122261.39250402014</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>122.26139250402014</v>
+      </c>
+      <c r="J7" s="18">
+        <f t="shared" si="2"/>
+        <v>3.0504940831543346</v>
+      </c>
+      <c r="K7" s="18">
+        <f t="shared" si="3"/>
+        <v>5.3899003396208567E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>95058.249836808158</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>95.058249836808159</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="2"/>
+        <v>2.9858885422966739</v>
+      </c>
+      <c r="K8" s="18">
+        <f t="shared" si="3"/>
+        <v>6.4605540857660682E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>74556.482886882673</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>74.556482886882677</v>
+      </c>
+      <c r="J9" s="18">
+        <f t="shared" si="2"/>
+        <v>2.9097283274643</v>
+      </c>
+      <c r="K9" s="18">
+        <f t="shared" si="3"/>
+        <v>7.6160214832373896E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>58963.308431392412</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>58.963308431392413</v>
+      </c>
+      <c r="J10" s="18">
+        <f t="shared" si="2"/>
+        <v>2.821484674233258</v>
+      </c>
+      <c r="K10" s="18">
+        <f t="shared" si="3"/>
+        <v>8.8243653231041996E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J11" s="18">
+        <f t="shared" si="2"/>
+        <v>2.7210526315789472</v>
+      </c>
+      <c r="K11" s="18">
+        <f t="shared" si="3"/>
+        <v>0.10043204265431083</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>37745.411867560397</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>37.745411867560399</v>
+      </c>
+      <c r="J12" s="18">
+        <f t="shared" si="2"/>
+        <v>2.6088341118192102</v>
+      </c>
+      <c r="K12" s="18">
+        <f t="shared" si="3"/>
+        <v>0.11221851975973696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>35</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>30529.696169372415</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>30.529696169372414</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" si="2"/>
+        <v>2.4857822012261335</v>
+      </c>
+      <c r="K13" s="18">
+        <f t="shared" si="3"/>
+        <v>0.12305191059307674</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>24861.344964843425</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>24.861344964843425</v>
+      </c>
+      <c r="J14" s="18">
+        <f t="shared" si="2"/>
+        <v>2.3533928041709387</v>
+      </c>
+      <c r="K14" s="18">
+        <f t="shared" si="3"/>
+        <v>0.13238939705519481</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>45</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>20376.600055247116</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>20.376600055247117</v>
+      </c>
+      <c r="J15" s="18">
+        <f t="shared" si="2"/>
+        <v>2.2136374729238422</v>
+      </c>
+      <c r="K15" s="18">
+        <f t="shared" si="3"/>
+        <v>0.13975533124709649</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>16804.033001084066</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>16.804033001084065</v>
+      </c>
+      <c r="J16" s="18">
+        <f t="shared" si="2"/>
+        <v>2.0688419873731188</v>
+      </c>
+      <c r="K16" s="18">
+        <f t="shared" si="3"/>
+        <v>0.14479548555072341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>55</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>13939.51662575143</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>13.93951662575143</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" si="2"/>
+        <v>1.9215260518459123</v>
+      </c>
+      <c r="K17" s="18">
+        <f t="shared" si="3"/>
+        <v>0.14731593552720645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>11628.382647478744</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>11.628382647478745</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="2"/>
+        <v>1.7742271052871876</v>
+      </c>
+      <c r="K18" s="18">
+        <f t="shared" si="3"/>
+        <v>0.14729894655872466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>65</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>9752.594274415751</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>9.7525942744157508</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="2"/>
+        <v>1.629333375578784</v>
+      </c>
+      <c r="K19" s="18">
+        <f t="shared" si="3"/>
+        <v>0.14489372970840364</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>70</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>8221.4492561069364</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>8.2214492561069363</v>
+      </c>
+      <c r="J20" s="18">
+        <f t="shared" si="2"/>
+        <v>1.4889475674422539</v>
+      </c>
+      <c r="K20" s="18">
+        <f t="shared" si="3"/>
+        <v>0.14038580813653012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>75</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="0"/>
+        <v>6964.7892094082217</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>6.964789209408222</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" si="2"/>
+        <v>1.3547945752429937</v>
+      </c>
+      <c r="K21" s="18">
+        <f t="shared" si="3"/>
+        <v>0.13415299219926013</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22">
+        <v>0.01</v>
+      </c>
+      <c r="G22">
+        <v>80</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="0"/>
+        <v>5928.0024974915805</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>5.9280024974915806</v>
+      </c>
+      <c r="J22" s="18">
+        <f t="shared" si="2"/>
+        <v>1.2281771204394902</v>
+      </c>
+      <c r="K22" s="18">
+        <f t="shared" si="3"/>
+        <v>0.1266174548035035</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <f>B21^2*B22</f>
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>85</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="0"/>
+        <v>5068.3205570363607</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>5.068320557036361</v>
+      </c>
+      <c r="J23" s="18">
+        <f t="shared" si="2"/>
+        <v>1.1099749155794145</v>
+      </c>
+      <c r="K23" s="18">
+        <f t="shared" si="3"/>
+        <v>0.11820220486007571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24">
+        <f>1.5*B21*B22</f>
+        <v>0.3</v>
+      </c>
+      <c r="G24">
+        <v>90</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>4352.0539530379674</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>4.3520539530379674</v>
+      </c>
+      <c r="J24" s="18">
+        <f t="shared" si="2"/>
+        <v>1.0006775400942014</v>
+      </c>
+      <c r="K24" s="18">
+        <f t="shared" si="3"/>
+        <v>0.10929737548521312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>95</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="0"/>
+        <v>3752.5160546369971</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>3.7525160546369971</v>
+      </c>
+      <c r="J25" s="18">
+        <f t="shared" si="2"/>
+        <v>0.90043908555385799</v>
+      </c>
+      <c r="K25" s="18">
+        <f t="shared" si="3"/>
+        <v>0.10023845454034341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <f>B24*B25</f>
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="0"/>
+        <v>3248.4533202316661</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>3.2484533202316661</v>
+      </c>
+      <c r="J26" s="18">
+        <f t="shared" si="2"/>
+        <v>0.80914320318389032</v>
+      </c>
+      <c r="K26" s="18">
+        <f t="shared" si="3"/>
+        <v>9.1295882369967662E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>105</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="0"/>
+        <v>2822.8513012688131</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>2.822851301268813</v>
+      </c>
+      <c r="J27" s="18">
+        <f t="shared" si="2"/>
+        <v>0.72646941583618996</v>
+      </c>
+      <c r="K27" s="18">
+        <f t="shared" si="3"/>
+        <v>8.2673787347700367E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28">
+        <f>3.3/(2^12)</f>
+        <v>8.0566406249999996E-4</v>
+      </c>
+      <c r="G28">
+        <v>110</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="0"/>
+        <v>2462.0210683801752</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>2.4620210683801753</v>
+      </c>
+      <c r="J28" s="18">
+        <f t="shared" si="2"/>
+        <v>0.65195440459246712</v>
+      </c>
+      <c r="K28" s="18">
+        <f t="shared" si="3"/>
+        <v>7.451501124372284E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29">
+        <f>B28/B26*B21</f>
+        <v>5.3710937499999991E-3</v>
+      </c>
+      <c r="G29">
+        <v>115</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="0"/>
+        <v>2154.896220150963</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>2.1548962201509632</v>
+      </c>
+      <c r="J29" s="18">
+        <f t="shared" si="2"/>
+        <v>0.58504469291222438</v>
+      </c>
+      <c r="K29" s="18">
+        <f t="shared" si="3"/>
+        <v>6.6909711680242734E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>120</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="0"/>
+        <v>1892.4889652740985</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>1.8924889652740986</v>
+      </c>
+      <c r="J30" s="18">
+        <f t="shared" si="2"/>
+        <v>0.52513932143561037</v>
+      </c>
+      <c r="K30" s="18">
+        <f t="shared" si="3"/>
+        <v>5.9905371476614011E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>125</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="0"/>
+        <v>1667.4670548512261</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>1.667467054851226</v>
+      </c>
+      <c r="J31" s="18">
+        <f t="shared" si="2"/>
+        <v>0.47162261141513984</v>
+      </c>
+      <c r="K31" s="18">
+        <f t="shared" si="3"/>
+        <v>5.3516710020470537E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>130</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="0"/>
+        <v>1473.8230325214975</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>1.4738230325214974</v>
+      </c>
+      <c r="J32" s="18">
+        <f t="shared" si="2"/>
+        <v>0.42388800956189304</v>
+      </c>
+      <c r="K32" s="18">
+        <f t="shared" si="3"/>
+        <v>4.7734601853246794E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>59</v>
+      </c>
+      <c r="K34" s="18">
+        <f>MIN(K3:K32)</f>
+        <v>2.23438106592182E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C55C07E-DD8A-4A57-9D3A-1D9832BE168C}">
+  <dimension ref="A12:B20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <f>B12^2*B13</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <f>1.5*B12*B13</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <f>B15*B16</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <f>3.3/(2^12)</f>
+        <v>8.0566406249999996E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20">
+        <f>B19/B17*B12</f>
+        <v>5.3710937499999991E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
footprints added, cap values corrected
</commit_message>
<xml_diff>
--- a/driver_module_calc.xlsx
+++ b/driver_module_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Documents\GitHub\TEMiWCZ_BLDC_HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C130EE-7433-4E73-B801-A5969F9ECA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E7A463-50AD-412E-BC66-6CDAE0CCE284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>Qg</t>
   </si>
@@ -230,23 +230,45 @@
     <t>TI BUCK GUIDES</t>
   </si>
   <si>
-    <t>https://www.tme.eu/pl/details/lm5007mmx_nopb/regulatory-napiecia-uklady-dc-dc/texas-instruments/</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/lm5007.pdf?ts=1728499998811&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FLM5007</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/pl/details/lm5085my_nopb/regulatory-napiecia-uklady-dc-dc/texas-instruments/</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/lm5085.pdf?ts=1728473150271&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FLM5085%253Futm_source%253Dgoogle%2526utm_medium%253Dcpc%2526utm_campaign%253Dapp-null-null-GPN_EN-cpc-pf-google-wwe%2526utm_content%253DLM5085%2526ds_k%253DLM5085%2526DCM%253Dyes%2526gad_source%253D1%2526gclid%253DEAIaIQobChMI4L7smpiBiQMV8xoGAB1X0xBfEAAYASAAEgK4wPD_BwE%2526gclsrc%253Daw.ds</t>
+    <t>https://www.ti.com/lit/ds/symlink/lmr51610.pdf?ts=1744201861273&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FLMR51610%253FkeyMatch%253Dlm51610%2526tisearch%253Duniversal_search</t>
+  </si>
+  <si>
+    <t>https://www.mouser.pl/ProductDetail/Texas-Instruments/LMR51610YDBVR?qs=sGAEpiMZZMvAX9OfPh%252B2NSM3AxpIzmi00gYVKQJvqx%2F6GBd8VBMoTw%3D%3D</t>
+  </si>
+  <si>
+    <t>LMR51610YDBVR</t>
+  </si>
+  <si>
+    <t>I_OUT</t>
+  </si>
+  <si>
+    <t>V_OUT</t>
+  </si>
+  <si>
+    <t>V_IN</t>
+  </si>
+  <si>
+    <t>L_MIN</t>
+  </si>
+  <si>
+    <t>F_SW</t>
+  </si>
+  <si>
+    <t>K_IND</t>
+  </si>
+  <si>
+    <t>R_FBT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_-* #,##0.000000000000_-;\-* #,##0.000000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +298,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -413,11 +450,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -439,8 +478,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Dziesiętny" xfId="2" builtinId="3"/>
+    <cellStyle name="Hiperłącze" xfId="3" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -3304,45 +3351,107 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15064B3A-5996-4225-AAD3-3A12E99682F8}">
-  <dimension ref="B2:B12"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
         <v>65</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18">
+        <f>((C13-C12)/(C11*C15))*(C12/(C13*C14))</f>
+        <v>1.3573232323232325E-5</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="24">
+        <v>1.3573232323232325E-5</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{B85B539A-D2FF-4DB1-BDBA-3E35446DDACC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
buck changed and calculated
</commit_message>
<xml_diff>
--- a/driver_module_calc.xlsx
+++ b/driver_module_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Documents\GitHub\TEMiWCZ_BLDC_HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E7A463-50AD-412E-BC66-6CDAE0CCE284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E530015-3AAA-4274-BE4E-574A5A8293C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>Qg</t>
   </si>
@@ -258,15 +258,49 @@
   </si>
   <si>
     <t>R_FBT</t>
+  </si>
+  <si>
+    <t>V_REF</t>
+  </si>
+  <si>
+    <t>R_FBB</t>
+  </si>
+  <si>
+    <t>[H]</t>
+  </si>
+  <si>
+    <t>[V]</t>
+  </si>
+  <si>
+    <t>[Ohm]</t>
+  </si>
+  <si>
+    <t>[A]</t>
+  </si>
+  <si>
+    <t>[Hz]</t>
+  </si>
+  <si>
+    <t>∆ iL</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R_ENB</t>
+  </si>
+  <si>
+    <t>R_ENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="_-* #,##0.000000000000_-;\-* #,##0.000000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="198" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??????????\ _z_ł_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -324,7 +358,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -449,6 +483,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -456,7 +505,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -483,7 +532,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dziesiętny" xfId="2" builtinId="3"/>
@@ -3351,102 +3410,176 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15064B3A-5996-4225-AAD3-3A12E99682F8}">
-  <dimension ref="B2:F21"/>
+  <dimension ref="B2:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="25">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="D11" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="28">
+        <f>C18</f>
+        <v>1.3573232323232325E-5</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="25"/>
+      <c r="P11" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="25">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="D12" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="25">
+        <v>22100</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="O12" s="25"/>
+      <c r="P12" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="25">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+      <c r="D13" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="25">
         <v>1100000</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="D14" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="27">
         <v>0.3</v>
       </c>
+      <c r="D15" s="25"/>
       <c r="E15" s="23"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="25">
         <f>((C13-C12)/(C11*C15))*(C12/(C13*C14))</f>
         <v>1.3573232323232325E-5</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="D18" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="24" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="24">
-        <v>1.3573232323232325E-5</v>
-      </c>
+      <c r="G18" s="25">
+        <f>((C12-G11)/G11)*G12</f>
+        <v>116025</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="29">
+        <f>(C12*(C13-C12))/(C13*K11*C14)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="30"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
fuses and missing footprints added, labels cleaned
</commit_message>
<xml_diff>
--- a/driver_module_calc.xlsx
+++ b/driver_module_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Documents\GitHub\TEMiWCZ_BLDC_HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E530015-3AAA-4274-BE4E-574A5A8293C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6B076A-4F49-4170-B0CD-E3ECFFCE8AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -299,8 +299,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="198" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??????????\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??????????\ _z_ł_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -540,8 +540,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -3413,7 +3413,7 @@
   <dimension ref="B2:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>